<commit_message>
update: new csv parse package, with action types added add: choice tip display add: choice prepare events
</commit_message>
<xml_diff>
--- a/Assets/Resources/Data/Card.xlsx
+++ b/Assets/Resources/Data/Card.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18450"/>
+    <workbookView windowHeight="18030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>ID</t>
   </si>
@@ -93,12 +93,12 @@
     <t>Left Next Card</t>
   </si>
   <si>
+    <t>Left Event</t>
+  </si>
+  <si>
     <t>Right Next Card</t>
   </si>
   <si>
-    <t>Left Event</t>
-  </si>
-  <si>
     <t>Right Event</t>
   </si>
   <si>
@@ -108,7 +108,10 @@
     <t>string</t>
   </si>
   <si>
-    <t>array&lt;enum&lt;none&gt;&gt;</t>
+    <t>action&lt;none&lt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>ref&lt;Left Event&gt;</t>
   </si>
   <si>
     <t>prologue</t>
@@ -198,7 +201,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,7 +209,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,47 +230,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,11 +245,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -306,21 +292,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,6 +365,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -392,19 +443,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,13 +491,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,37 +503,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,42 +516,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,6 +556,60 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -575,37 +632,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,30 +651,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -661,145 +664,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1164,7 +1167,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -1173,8 +1176,9 @@
     <col min="2" max="2" width="29.375" customWidth="1"/>
     <col min="3" max="3" width="20.125" customWidth="1"/>
     <col min="4" max="4" width="24.625" customWidth="1"/>
-    <col min="5" max="6" width="19.125" customWidth="1"/>
-    <col min="7" max="7" width="27.25" customWidth="1"/>
+    <col min="5" max="5" width="19.125" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="7" width="19.125" customWidth="1"/>
     <col min="8" max="8" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1221,109 +1225,109 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
+      <c r="G5" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
       <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
+      <c r="G7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>